<commit_message>
Intermediate commit to preserve progress.
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCF0618-6291-E046-9D11-CBDB33B2DBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BDC708-D2D1-5C4F-B043-C66D65060835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="460" windowWidth="22140" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6440" yWindow="460" windowWidth="32860" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
     <sheet name="strategy_id-1" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$512</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="717">
   <si>
     <t>subsector</t>
   </si>
@@ -2616,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS667"/>
+  <dimension ref="A1:AT667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A655" zoomScale="119" workbookViewId="0">
-      <selection activeCell="B667" sqref="B667"/>
+    <sheetView tabSelected="1" topLeftCell="A646" zoomScale="119" workbookViewId="0">
+      <selection activeCell="A668" sqref="A668:XFD678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -82874,7 +82875,7 @@
         <v>0.12122999821135493</v>
       </c>
     </row>
-    <row r="657" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>48</v>
       </c>
@@ -82996,7 +82997,7 @@
         <v>0.176479365113832</v>
       </c>
     </row>
-    <row r="658" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
         <v>48</v>
       </c>
@@ -83118,7 +83119,7 @@
         <v>0.26119171237428684</v>
       </c>
     </row>
-    <row r="659" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
         <v>48</v>
       </c>
@@ -83240,7 +83241,7 @@
         <v>0.14974831158375401</v>
       </c>
     </row>
-    <row r="660" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
         <v>48</v>
       </c>
@@ -83362,7 +83363,7 @@
         <v>0.17895541881894148</v>
       </c>
     </row>
-    <row r="661" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>48</v>
       </c>
@@ -83484,7 +83485,7 @@
         <v>0.2625753407614892</v>
       </c>
     </row>
-    <row r="662" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
         <v>48</v>
       </c>
@@ -83606,7 +83607,7 @@
         <v>0.21859292392490642</v>
       </c>
     </row>
-    <row r="663" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
         <v>48</v>
       </c>
@@ -83728,7 +83729,7 @@
         <v>0.19787599508057382</v>
       </c>
     </row>
-    <row r="664" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
         <v>47</v>
       </c>
@@ -83850,7 +83851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="665" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
         <v>47</v>
       </c>
@@ -83972,7 +83973,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="666" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
         <v>47</v>
       </c>
@@ -84094,7 +84095,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="667" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
         <v>47</v>
       </c>
@@ -84214,6 +84215,10 @@
       </c>
       <c r="AS667">
         <v>1</v>
+      </c>
+      <c r="AT667" t="e">
+        <f>#REF!*1.25</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -84498,4 +84503,278 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60261E01-9474-4248-B06C-26457F8C015B}">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>713</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1.01</v>
+      </c>
+      <c r="O2">
+        <v>1.02</v>
+      </c>
+      <c r="P2">
+        <v>1.03</v>
+      </c>
+      <c r="Q2">
+        <v>1.04</v>
+      </c>
+      <c r="R2">
+        <v>1.05</v>
+      </c>
+      <c r="S2">
+        <v>1.06</v>
+      </c>
+      <c r="T2">
+        <v>1.07</v>
+      </c>
+      <c r="U2">
+        <v>1.08</v>
+      </c>
+      <c r="V2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="W2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Y2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Z2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AA2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AC2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AD2">
+        <v>1.17</v>
+      </c>
+      <c r="AE2">
+        <v>1.18</v>
+      </c>
+      <c r="AF2">
+        <v>1.19</v>
+      </c>
+      <c r="AG2">
+        <v>1.2</v>
+      </c>
+      <c r="AH2">
+        <v>1.21</v>
+      </c>
+      <c r="AI2">
+        <v>1.22</v>
+      </c>
+      <c r="AJ2">
+        <v>1.23</v>
+      </c>
+      <c r="AK2">
+        <v>1.24</v>
+      </c>
+      <c r="AL2">
+        <v>1.25</v>
+      </c>
+      <c r="AM2">
+        <v>1.25</v>
+      </c>
+      <c r="AN2">
+        <v>1.25</v>
+      </c>
+      <c r="AO2">
+        <v>1.25</v>
+      </c>
+      <c r="AP2">
+        <v>1.25</v>
+      </c>
+      <c r="AQ2">
+        <v>1.25</v>
+      </c>
+      <c r="AR2">
+        <v>1.25</v>
+      </c>
+      <c r="AS2">
+        <v>1.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Intermediate preservation. Fixed bug in sampling_units.py. Completed SISEPUEDEoutputDatabase.
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BDC708-D2D1-5C4F-B043-C66D65060835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05365B84-11FF-A048-B596-6CEFF069A6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="460" windowWidth="32860" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="460" windowWidth="32860" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="strategy_id-2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$512</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$667</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2617,10 +2617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT667"/>
+  <dimension ref="A1:AS667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A646" zoomScale="119" workbookViewId="0">
-      <selection activeCell="A668" sqref="A668:XFD678"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B668" sqref="B668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6189,6 +6190,9 @@
       <c r="B30" s="3" t="s">
         <v>649</v>
       </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
       <c r="G30">
         <v>1</v>
       </c>
@@ -6314,6 +6318,9 @@
       <c r="B31" s="3" t="s">
         <v>650</v>
       </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
       <c r="G31">
         <v>1</v>
       </c>
@@ -6439,6 +6446,9 @@
       <c r="B32" s="3" t="s">
         <v>651</v>
       </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
       <c r="G32">
         <v>1</v>
       </c>
@@ -6564,6 +6574,9 @@
       <c r="B33" s="3" t="s">
         <v>652</v>
       </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
       <c r="G33">
         <v>1</v>
       </c>
@@ -6689,6 +6702,9 @@
       <c r="B34" s="3" t="s">
         <v>653</v>
       </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
@@ -12304,6 +12320,9 @@
       <c r="B80" s="3" t="s">
         <v>561</v>
       </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
       <c r="G80">
         <v>1</v>
       </c>
@@ -12429,6 +12448,9 @@
       <c r="B81" s="3" t="s">
         <v>562</v>
       </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
       <c r="G81">
         <v>1</v>
       </c>
@@ -12554,6 +12576,9 @@
       <c r="B82" s="3" t="s">
         <v>563</v>
       </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
       <c r="G82">
         <v>1</v>
       </c>
@@ -12679,6 +12704,9 @@
       <c r="B83" s="3" t="s">
         <v>564</v>
       </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
       <c r="G83">
         <v>1</v>
       </c>
@@ -12804,6 +12832,9 @@
       <c r="B84" s="3" t="s">
         <v>565</v>
       </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
       <c r="G84">
         <v>1</v>
       </c>
@@ -12929,6 +12960,9 @@
       <c r="B85" s="3" t="s">
         <v>566</v>
       </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
       <c r="G85">
         <v>1</v>
       </c>
@@ -13054,6 +13088,9 @@
       <c r="B86" s="3" t="s">
         <v>567</v>
       </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
       <c r="G86">
         <v>1</v>
       </c>
@@ -13179,6 +13216,9 @@
       <c r="B87" s="3" t="s">
         <v>568</v>
       </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
       <c r="G87">
         <v>1</v>
       </c>
@@ -13304,6 +13344,9 @@
       <c r="B88" s="3" t="s">
         <v>569</v>
       </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
       <c r="G88">
         <v>1</v>
       </c>
@@ -13429,6 +13472,9 @@
       <c r="B89" s="3" t="s">
         <v>570</v>
       </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
       <c r="G89">
         <v>1</v>
       </c>
@@ -17580,6 +17626,9 @@
       <c r="B123" s="2" t="s">
         <v>571</v>
       </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
       <c r="G123">
         <v>1</v>
       </c>
@@ -17705,6 +17754,9 @@
       <c r="B124" s="2" t="s">
         <v>572</v>
       </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
       <c r="G124">
         <v>1</v>
       </c>
@@ -17830,6 +17882,9 @@
       <c r="B125" s="2" t="s">
         <v>573</v>
       </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
       <c r="G125">
         <v>1</v>
       </c>
@@ -17955,6 +18010,9 @@
       <c r="B126" s="2" t="s">
         <v>574</v>
       </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
       <c r="G126">
         <v>1</v>
       </c>
@@ -18080,6 +18138,9 @@
       <c r="B127" s="2" t="s">
         <v>575</v>
       </c>
+      <c r="F127">
+        <v>1</v>
+      </c>
       <c r="G127">
         <v>1</v>
       </c>
@@ -18205,6 +18266,9 @@
       <c r="B128" s="2" t="s">
         <v>576</v>
       </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
       <c r="G128">
         <v>1</v>
       </c>
@@ -18330,6 +18394,9 @@
       <c r="B129" s="2" t="s">
         <v>577</v>
       </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
       <c r="G129">
         <v>1</v>
       </c>
@@ -18455,6 +18522,9 @@
       <c r="B130" s="2" t="s">
         <v>578</v>
       </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
       <c r="G130">
         <v>1</v>
       </c>
@@ -18580,6 +18650,9 @@
       <c r="B131" s="2" t="s">
         <v>579</v>
       </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
       <c r="G131">
         <v>1</v>
       </c>
@@ -18705,6 +18778,9 @@
       <c r="B132" s="2" t="s">
         <v>580</v>
       </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
       <c r="G132">
         <v>1</v>
       </c>
@@ -18830,6 +18906,9 @@
       <c r="B133" s="2" t="s">
         <v>581</v>
       </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
       <c r="G133">
         <v>1</v>
       </c>
@@ -18955,6 +19034,9 @@
       <c r="B134" s="2" t="s">
         <v>582</v>
       </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
       <c r="G134">
         <v>1</v>
       </c>
@@ -19080,6 +19162,9 @@
       <c r="B135" s="2" t="s">
         <v>583</v>
       </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
       <c r="G135">
         <v>1</v>
       </c>
@@ -19205,6 +19290,9 @@
       <c r="B136" s="2" t="s">
         <v>584</v>
       </c>
+      <c r="F136">
+        <v>1</v>
+      </c>
       <c r="G136">
         <v>1</v>
       </c>
@@ -19330,6 +19418,9 @@
       <c r="B137" s="2" t="s">
         <v>585</v>
       </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
       <c r="G137">
         <v>1</v>
       </c>
@@ -19455,6 +19546,9 @@
       <c r="B138" s="2" t="s">
         <v>586</v>
       </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
       <c r="G138">
         <v>1</v>
       </c>
@@ -19580,6 +19674,9 @@
       <c r="B139" s="2" t="s">
         <v>587</v>
       </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
       <c r="G139">
         <v>1</v>
       </c>
@@ -19705,6 +19802,9 @@
       <c r="B140" s="2" t="s">
         <v>588</v>
       </c>
+      <c r="F140">
+        <v>1</v>
+      </c>
       <c r="G140">
         <v>1</v>
       </c>
@@ -19830,6 +19930,9 @@
       <c r="B141" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="F141">
+        <v>1</v>
+      </c>
       <c r="G141">
         <v>1</v>
       </c>
@@ -19955,6 +20058,9 @@
       <c r="B142" s="2" t="s">
         <v>590</v>
       </c>
+      <c r="F142">
+        <v>1</v>
+      </c>
       <c r="G142">
         <v>1</v>
       </c>
@@ -61316,6 +61422,9 @@
       <c r="B481" s="2" t="s">
         <v>353</v>
       </c>
+      <c r="F481">
+        <v>1</v>
+      </c>
       <c r="G481">
         <v>1</v>
       </c>
@@ -61441,6 +61550,9 @@
       <c r="B482" s="2" t="s">
         <v>354</v>
       </c>
+      <c r="F482">
+        <v>1</v>
+      </c>
       <c r="G482">
         <v>1</v>
       </c>
@@ -61566,6 +61678,9 @@
       <c r="B483" s="2" t="s">
         <v>355</v>
       </c>
+      <c r="F483">
+        <v>1</v>
+      </c>
       <c r="G483">
         <v>1</v>
       </c>
@@ -61691,6 +61806,9 @@
       <c r="B484" s="2" t="s">
         <v>356</v>
       </c>
+      <c r="F484">
+        <v>1</v>
+      </c>
       <c r="G484">
         <v>1</v>
       </c>
@@ -61816,6 +61934,9 @@
       <c r="B485" s="2" t="s">
         <v>357</v>
       </c>
+      <c r="F485">
+        <v>1</v>
+      </c>
       <c r="G485">
         <v>1</v>
       </c>
@@ -61941,6 +62062,9 @@
       <c r="B486" s="2" t="s">
         <v>358</v>
       </c>
+      <c r="F486">
+        <v>1</v>
+      </c>
       <c r="G486">
         <v>1</v>
       </c>
@@ -62066,6 +62190,9 @@
       <c r="B487" s="2" t="s">
         <v>359</v>
       </c>
+      <c r="F487">
+        <v>1</v>
+      </c>
       <c r="G487">
         <v>1</v>
       </c>
@@ -62191,6 +62318,9 @@
       <c r="B488" s="2" t="s">
         <v>360</v>
       </c>
+      <c r="F488">
+        <v>1</v>
+      </c>
       <c r="G488">
         <v>1</v>
       </c>
@@ -62316,6 +62446,9 @@
       <c r="B489" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="F489">
+        <v>1</v>
+      </c>
       <c r="G489">
         <v>1</v>
       </c>
@@ -71592,6 +71725,9 @@
       <c r="B565" s="2" t="s">
         <v>411</v>
       </c>
+      <c r="F565">
+        <v>1</v>
+      </c>
       <c r="G565">
         <v>1</v>
       </c>
@@ -72571,6 +72707,9 @@
       <c r="B573" s="2" t="s">
         <v>490</v>
       </c>
+      <c r="F573">
+        <v>1</v>
+      </c>
       <c r="G573">
         <v>1</v>
       </c>
@@ -72696,6 +72835,9 @@
       <c r="B574" s="2" t="s">
         <v>491</v>
       </c>
+      <c r="F574">
+        <v>1</v>
+      </c>
       <c r="G574">
         <v>1</v>
       </c>
@@ -72821,6 +72963,9 @@
       <c r="B575" s="2" t="s">
         <v>496</v>
       </c>
+      <c r="F575">
+        <v>1</v>
+      </c>
       <c r="G575">
         <v>1</v>
       </c>
@@ -72946,6 +73091,9 @@
       <c r="B576" s="2" t="s">
         <v>492</v>
       </c>
+      <c r="F576">
+        <v>1</v>
+      </c>
       <c r="G576">
         <v>1</v>
       </c>
@@ -73071,6 +73219,9 @@
       <c r="B577" s="2" t="s">
         <v>493</v>
       </c>
+      <c r="F577">
+        <v>1</v>
+      </c>
       <c r="G577">
         <v>1</v>
       </c>
@@ -73196,6 +73347,9 @@
       <c r="B578" s="2" t="s">
         <v>607</v>
       </c>
+      <c r="F578">
+        <v>1</v>
+      </c>
       <c r="G578">
         <v>1</v>
       </c>
@@ -73321,6 +73475,9 @@
       <c r="B579" s="2" t="s">
         <v>608</v>
       </c>
+      <c r="F579">
+        <v>1</v>
+      </c>
       <c r="G579">
         <v>1</v>
       </c>
@@ -73446,6 +73603,9 @@
       <c r="B580" s="2" t="s">
         <v>609</v>
       </c>
+      <c r="F580">
+        <v>1</v>
+      </c>
       <c r="G580">
         <v>1</v>
       </c>
@@ -73571,6 +73731,9 @@
       <c r="B581" s="2" t="s">
         <v>610</v>
       </c>
+      <c r="F581">
+        <v>1</v>
+      </c>
       <c r="G581">
         <v>1</v>
       </c>
@@ -73696,6 +73859,9 @@
       <c r="B582" s="2" t="s">
         <v>611</v>
       </c>
+      <c r="F582">
+        <v>1</v>
+      </c>
       <c r="G582">
         <v>1</v>
       </c>
@@ -73821,6 +73987,9 @@
       <c r="B583" s="2" t="s">
         <v>497</v>
       </c>
+      <c r="F583">
+        <v>1</v>
+      </c>
       <c r="G583">
         <v>1</v>
       </c>
@@ -73946,6 +74115,9 @@
       <c r="B584" s="2" t="s">
         <v>498</v>
       </c>
+      <c r="F584">
+        <v>1</v>
+      </c>
       <c r="G584">
         <v>1</v>
       </c>
@@ -74071,6 +74243,9 @@
       <c r="B585" s="2" t="s">
         <v>494</v>
       </c>
+      <c r="F585">
+        <v>1</v>
+      </c>
       <c r="G585">
         <v>1</v>
       </c>
@@ -74196,6 +74371,9 @@
       <c r="B586" s="2" t="s">
         <v>495</v>
       </c>
+      <c r="F586">
+        <v>1</v>
+      </c>
       <c r="G586">
         <v>1</v>
       </c>
@@ -74321,6 +74499,9 @@
       <c r="B587" s="2" t="s">
         <v>446</v>
       </c>
+      <c r="F587">
+        <v>1</v>
+      </c>
       <c r="G587">
         <v>1</v>
       </c>
@@ -75056,6 +75237,9 @@
       <c r="B593" s="2" t="s">
         <v>502</v>
       </c>
+      <c r="F593">
+        <v>1</v>
+      </c>
       <c r="G593">
         <v>1</v>
       </c>
@@ -75181,6 +75365,9 @@
       <c r="B594" s="2" t="s">
         <v>503</v>
       </c>
+      <c r="F594">
+        <v>1</v>
+      </c>
       <c r="G594">
         <v>1</v>
       </c>
@@ -75306,6 +75493,9 @@
       <c r="B595" s="2" t="s">
         <v>500</v>
       </c>
+      <c r="F595">
+        <v>1</v>
+      </c>
       <c r="G595">
         <v>1</v>
       </c>
@@ -75431,6 +75621,9 @@
       <c r="B596" s="2" t="s">
         <v>501</v>
       </c>
+      <c r="F596">
+        <v>1</v>
+      </c>
       <c r="G596">
         <v>1</v>
       </c>
@@ -75678,6 +75871,9 @@
       <c r="B598" s="2" t="s">
         <v>591</v>
       </c>
+      <c r="F598">
+        <v>1</v>
+      </c>
       <c r="G598">
         <v>1</v>
       </c>
@@ -75803,6 +75999,12 @@
       <c r="B599" s="2" t="s">
         <v>594</v>
       </c>
+      <c r="F599">
+        <v>1</v>
+      </c>
+      <c r="G599">
+        <v>1</v>
+      </c>
       <c r="H599">
         <v>0.16613924050632911</v>
       </c>
@@ -75925,6 +76127,12 @@
       <c r="B600" s="2" t="s">
         <v>595</v>
       </c>
+      <c r="F600">
+        <v>1</v>
+      </c>
+      <c r="G600">
+        <v>1</v>
+      </c>
       <c r="H600">
         <v>0.2412868632707775</v>
       </c>
@@ -76047,6 +76255,12 @@
       <c r="B601" s="2" t="s">
         <v>596</v>
       </c>
+      <c r="F601">
+        <v>1</v>
+      </c>
+      <c r="G601">
+        <v>1</v>
+      </c>
       <c r="H601">
         <v>0.28423772609819126</v>
       </c>
@@ -76169,6 +76383,12 @@
       <c r="B602" s="2" t="s">
         <v>597</v>
       </c>
+      <c r="F602">
+        <v>1</v>
+      </c>
+      <c r="G602">
+        <v>1</v>
+      </c>
       <c r="H602">
         <v>0.52765957446808509</v>
       </c>
@@ -76291,6 +76511,12 @@
       <c r="B603" s="2" t="s">
         <v>598</v>
       </c>
+      <c r="F603">
+        <v>1</v>
+      </c>
+      <c r="G603">
+        <v>1</v>
+      </c>
       <c r="H603">
         <v>0.52765957446808509</v>
       </c>
@@ -76413,6 +76639,9 @@
       <c r="B604" s="2" t="s">
         <v>592</v>
       </c>
+      <c r="F604">
+        <v>1</v>
+      </c>
       <c r="G604">
         <v>1</v>
       </c>
@@ -78124,6 +78353,12 @@
       <c r="B618" t="s">
         <v>664</v>
       </c>
+      <c r="F618">
+        <v>1</v>
+      </c>
+      <c r="G618">
+        <v>1</v>
+      </c>
       <c r="H618">
         <v>0.98477157360406087</v>
       </c>
@@ -82875,7 +83110,7 @@
         <v>0.12122999821135493</v>
       </c>
     </row>
-    <row r="657" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>48</v>
       </c>
@@ -82997,7 +83232,7 @@
         <v>0.176479365113832</v>
       </c>
     </row>
-    <row r="658" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
         <v>48</v>
       </c>
@@ -83119,7 +83354,7 @@
         <v>0.26119171237428684</v>
       </c>
     </row>
-    <row r="659" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
         <v>48</v>
       </c>
@@ -83241,7 +83476,7 @@
         <v>0.14974831158375401</v>
       </c>
     </row>
-    <row r="660" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
         <v>48</v>
       </c>
@@ -83363,7 +83598,7 @@
         <v>0.17895541881894148</v>
       </c>
     </row>
-    <row r="661" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>48</v>
       </c>
@@ -83485,7 +83720,7 @@
         <v>0.2625753407614892</v>
       </c>
     </row>
-    <row r="662" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
         <v>48</v>
       </c>
@@ -83607,7 +83842,7 @@
         <v>0.21859292392490642</v>
       </c>
     </row>
-    <row r="663" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
         <v>48</v>
       </c>
@@ -83729,7 +83964,7 @@
         <v>0.19787599508057382</v>
       </c>
     </row>
-    <row r="664" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
         <v>47</v>
       </c>
@@ -83851,12 +84086,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="665" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
         <v>47</v>
       </c>
       <c r="B665" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="H665">
         <v>1</v>
@@ -83973,12 +84208,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="666" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
         <v>47</v>
       </c>
       <c r="B666" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H666">
         <v>1</v>
@@ -84095,12 +84330,12 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="667" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
         <v>47</v>
       </c>
       <c r="B667" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="H667">
         <v>1</v>
@@ -84216,13 +84451,9 @@
       <c r="AS667">
         <v>1</v>
       </c>
-      <c r="AT667" t="e">
-        <f>#REF!*1.25</f>
-        <v>#REF!</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS512" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AS667" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS608">
     <sortCondition ref="A2:A608"/>
     <sortCondition ref="B2:B608"/>

</xml_diff>

<commit_message>
updated scripts to handle regions properly and updated reference tables
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14386BE5-645E-A44A-95AA-31C01A467E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9CECC8-A577-2F46-9A03-CB61464603BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="460" windowWidth="32860" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="32860" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$667</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$665</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="714">
   <si>
     <t>subsector</t>
   </si>
@@ -2176,13 +2176,7 @@
     <t>factor_lndu_soil_management_croplands</t>
   </si>
   <si>
-    <t>trajmax_factor_lndu_soil_management_grasslands</t>
-  </si>
-  <si>
-    <t>trajmin_factor_lndu_soil_management_grasslands</t>
-  </si>
-  <si>
-    <t>trajmix_factor_lndu_soil_management_grasslands</t>
+    <t>factor_lndu_soil_management_grasslands</t>
   </si>
 </sst>
 </file>
@@ -2612,11 +2606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS667"/>
+  <dimension ref="A1:AS665"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E653" sqref="E653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -84086,7 +84080,7 @@
         <v>46</v>
       </c>
       <c r="B665" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H665">
         <v>1</v>
@@ -84203,252 +84197,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="666" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A666" t="s">
-        <v>46</v>
-      </c>
-      <c r="B666" t="s">
-        <v>715</v>
-      </c>
-      <c r="H666">
-        <v>1</v>
-      </c>
-      <c r="I666">
-        <v>1</v>
-      </c>
-      <c r="J666">
-        <v>0</v>
-      </c>
-      <c r="K666">
-        <v>0</v>
-      </c>
-      <c r="L666">
-        <v>0</v>
-      </c>
-      <c r="M666">
-        <v>0.01</v>
-      </c>
-      <c r="N666">
-        <v>0.02</v>
-      </c>
-      <c r="O666">
-        <v>0.03</v>
-      </c>
-      <c r="P666">
-        <v>0.04</v>
-      </c>
-      <c r="Q666">
-        <v>0.05</v>
-      </c>
-      <c r="R666">
-        <v>0.06</v>
-      </c>
-      <c r="S666">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="T666">
-        <v>0.08</v>
-      </c>
-      <c r="U666">
-        <v>0.09</v>
-      </c>
-      <c r="V666">
-        <v>0.1</v>
-      </c>
-      <c r="W666">
-        <v>0.11</v>
-      </c>
-      <c r="X666">
-        <v>0.12</v>
-      </c>
-      <c r="Y666">
-        <v>0.13</v>
-      </c>
-      <c r="Z666">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="AA666">
-        <v>0.15</v>
-      </c>
-      <c r="AB666">
-        <v>0.16</v>
-      </c>
-      <c r="AC666">
-        <v>0.17</v>
-      </c>
-      <c r="AD666">
-        <v>0.18</v>
-      </c>
-      <c r="AE666">
-        <v>0.19</v>
-      </c>
-      <c r="AF666">
-        <v>0.2</v>
-      </c>
-      <c r="AG666">
-        <v>0.21</v>
-      </c>
-      <c r="AH666">
-        <v>0.22</v>
-      </c>
-      <c r="AI666">
-        <v>0.23</v>
-      </c>
-      <c r="AJ666">
-        <v>0.24</v>
-      </c>
-      <c r="AK666">
-        <v>0.25</v>
-      </c>
-      <c r="AL666">
-        <v>0.26</v>
-      </c>
-      <c r="AM666">
-        <v>0.27</v>
-      </c>
-      <c r="AN666">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="AO666">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AP666">
-        <v>0.3</v>
-      </c>
-      <c r="AQ666">
-        <v>0.31</v>
-      </c>
-      <c r="AR666">
-        <v>0.32</v>
-      </c>
-      <c r="AS666">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="667" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A667" t="s">
-        <v>46</v>
-      </c>
-      <c r="B667" t="s">
-        <v>713</v>
-      </c>
-      <c r="H667">
-        <v>1</v>
-      </c>
-      <c r="I667">
-        <v>1</v>
-      </c>
-      <c r="J667">
-        <v>0.9</v>
-      </c>
-      <c r="K667">
-        <v>0.9</v>
-      </c>
-      <c r="L667">
-        <v>0.9</v>
-      </c>
-      <c r="M667">
-        <v>0.9</v>
-      </c>
-      <c r="N667">
-        <v>0.9</v>
-      </c>
-      <c r="O667">
-        <v>0.9</v>
-      </c>
-      <c r="P667">
-        <v>0.9</v>
-      </c>
-      <c r="Q667">
-        <v>0.9</v>
-      </c>
-      <c r="R667">
-        <v>0.9</v>
-      </c>
-      <c r="S667">
-        <v>0.9</v>
-      </c>
-      <c r="T667">
-        <v>0.9</v>
-      </c>
-      <c r="U667">
-        <v>0.9</v>
-      </c>
-      <c r="V667">
-        <v>0.9</v>
-      </c>
-      <c r="W667">
-        <v>0.9</v>
-      </c>
-      <c r="X667">
-        <v>0.9</v>
-      </c>
-      <c r="Y667">
-        <v>0.9</v>
-      </c>
-      <c r="Z667">
-        <v>0.9</v>
-      </c>
-      <c r="AA667">
-        <v>0.9</v>
-      </c>
-      <c r="AB667">
-        <v>0.9</v>
-      </c>
-      <c r="AC667">
-        <v>0.9</v>
-      </c>
-      <c r="AD667">
-        <v>0.9</v>
-      </c>
-      <c r="AE667">
-        <v>0.9</v>
-      </c>
-      <c r="AF667">
-        <v>0.9</v>
-      </c>
-      <c r="AG667">
-        <v>0.9</v>
-      </c>
-      <c r="AH667">
-        <v>0.9</v>
-      </c>
-      <c r="AI667">
-        <v>0.91</v>
-      </c>
-      <c r="AJ667">
-        <v>0.92</v>
-      </c>
-      <c r="AK667">
-        <v>0.93</v>
-      </c>
-      <c r="AL667">
-        <v>0.94</v>
-      </c>
-      <c r="AM667">
-        <v>0.95</v>
-      </c>
-      <c r="AN667">
-        <v>0.96</v>
-      </c>
-      <c r="AO667">
-        <v>0.97</v>
-      </c>
-      <c r="AP667">
-        <v>0.98</v>
-      </c>
-      <c r="AQ667">
-        <v>0.99</v>
-      </c>
-      <c r="AR667">
-        <v>1</v>
-      </c>
-      <c r="AS667">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AS667" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AS665" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS608">
     <sortCondition ref="A2:A608"/>
     <sortCondition ref="B2:B608"/>

</xml_diff>